<commit_message>
Update Pinjaman dan Simpanan
</commit_message>
<xml_diff>
--- a/assets/template/Template_Saldo_pinjaman.xlsx
+++ b/assets/template/Template_Saldo_pinjaman.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\inkopkar\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6372B2A-2406-4EA7-9700-D2BC64BB214D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2DDFEE-607E-4EE7-9DC3-A917D8E1E1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2E8CD1E3-45E7-4754-8C58-5E9B6364AB8C}"/>
+    <workbookView xWindow="3204" yWindow="3204" windowWidth="17280" windowHeight="8880" xr2:uid="{2E8CD1E3-45E7-4754-8C58-5E9B6364AB8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nomor Anggota</t>
   </si>
@@ -83,10 +83,19 @@
     <t>Sisa Cicilan</t>
   </si>
   <si>
-    <t>CICILAN BULAN JULY 2025</t>
-  </si>
-  <si>
     <t>Tanggal Bayar</t>
+  </si>
+  <si>
+    <t>Bulan (Angka)</t>
+  </si>
+  <si>
+    <t>Jenis Pinjaman</t>
+  </si>
+  <si>
+    <t>PINJAMAN UANG</t>
+  </si>
+  <si>
+    <t>CICILAN BULAN SEPTEMBER 2025</t>
   </si>
 </sst>
 </file>
@@ -516,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0B6173-9C9B-4B37-B0E3-EBD30C0093EF}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,12 +536,14 @@
     <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
     <col min="6" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -546,17 +557,23 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3"/>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -567,35 +584,43 @@
         <v>10000000</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="5">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5">
         <v>1000000</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>9000000</v>
       </c>
-      <c r="G2" s="9">
+      <c r="H2" s="5">
+        <v>9</v>
+      </c>
+      <c r="I2" s="9">
         <f ca="1">TODAY()</f>
-        <v>45897</v>
-      </c>
-      <c r="H2" s="4" t="s">
+        <v>45904</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
+      <c r="J3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G5" s="8"/>
     </row>
   </sheetData>

</xml_diff>